<commit_message>
18 started a mind map to keep track of upgrades useing programe Xmind
</commit_message>
<xml_diff>
--- a/Tower Info.xlsx
+++ b/Tower Info.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\Documents\Unreal Projects\Test Project 01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F9E351-EFBD-4B13-9F86-75C77A0B76D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAF84A7-EB07-4473-9200-151477E88E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tower Base Traits" sheetId="1" r:id="rId1"/>
+    <sheet name="Tower components" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
   <si>
     <t>Tower Base Traits</t>
   </si>
@@ -96,9 +97,6 @@
     <t>water damage</t>
   </si>
   <si>
-    <t>air damage</t>
-  </si>
-  <si>
     <t>Poison damage</t>
   </si>
   <si>
@@ -169,6 +167,69 @@
   </si>
   <si>
     <t>Componets:</t>
+  </si>
+  <si>
+    <t>Name:</t>
+  </si>
+  <si>
+    <t>Most common demage from melee &amp; rnage</t>
+  </si>
+  <si>
+    <t>Resistance to Poison damage</t>
+  </si>
+  <si>
+    <t>Resistance to Corruption damage</t>
+  </si>
+  <si>
+    <t>Magic damage is made up by Fire, earth, water &amp; air e.g a fire spell could be made 85% FD then 5% ED 5% WD &amp; 5% AD</t>
+  </si>
+  <si>
+    <t>Resistance to fire damage</t>
+  </si>
+  <si>
+    <t>Resistance to earth damage</t>
+  </si>
+  <si>
+    <t>Resistance to water damage</t>
+  </si>
+  <si>
+    <t>Resistance to air damage</t>
+  </si>
+  <si>
+    <t>Air damage</t>
+  </si>
+  <si>
+    <t>Ability Traits:</t>
+  </si>
+  <si>
+    <t>Make resource</t>
+  </si>
+  <si>
+    <t>Buff towers</t>
+  </si>
+  <si>
+    <t>Shield tower</t>
+  </si>
+  <si>
+    <t>Spawn creeps</t>
+  </si>
+  <si>
+    <t>Debuff enemies</t>
+  </si>
+  <si>
+    <t>The tower can make resources</t>
+  </si>
+  <si>
+    <t>The tower can buff itself or others</t>
+  </si>
+  <si>
+    <t>The tower can Shield itself or others</t>
+  </si>
+  <si>
+    <t>The tower can spawn creeps</t>
+  </si>
+  <si>
+    <t>The tower can debuff enemies in some way</t>
   </si>
 </sst>
 </file>
@@ -192,7 +253,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="6"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -287,7 +348,49 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -295,53 +398,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -623,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Q22"/>
+  <dimension ref="B1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,304 +698,502 @@
     <col min="11" max="11" width="10.109375" customWidth="1"/>
     <col min="14" max="14" width="13.77734375" customWidth="1"/>
     <col min="17" max="17" width="9.88671875" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" customWidth="1"/>
+    <col min="23" max="23" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="4" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="4" spans="2:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+    </row>
+    <row r="6" spans="2:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="16" t="s">
+      <c r="F6" s="6"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="N5" t="s">
+      <c r="O6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="7" t="s">
+      <c r="O7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="N6" t="s">
+      <c r="J8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="O8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="P8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W8" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W9" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="7" t="s">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="N7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="J10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W10" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="7" t="s">
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="13"/>
+    </row>
+    <row r="12" spans="2:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="N8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="J12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="7" t="s">
+      <c r="P12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="13"/>
+    </row>
+    <row r="13" spans="2:23" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="N9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="N10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="N11" t="s">
+      <c r="J13" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="18" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="18"/>
-    </row>
-    <row r="21" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="19" t="s">
-        <v>44</v>
-      </c>
+      <c r="K13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{835DB90F-02B5-433E-BF37-83E02E0A67CF}">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="19"/>
+    </row>
+    <row r="5" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
20 Updates tower spreedsheet, changed tower slection and tower spawning as well as bugs with red highlight
</commit_message>
<xml_diff>
--- a/Tower Info.xlsx
+++ b/Tower Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\Documents\Unreal Projects\Test Project 01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEB4D68-ED00-41EE-9A8A-E797AEA42F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C218D5-D912-49B5-9B04-50B9255A1A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tower Base Traits" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="69">
   <si>
     <t>Tower Base Traits</t>
   </si>
@@ -233,6 +233,15 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Spawner</t>
+  </si>
+  <si>
+    <t>Reflex Damage</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -348,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -362,11 +371,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -377,9 +383,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -387,9 +390,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -689,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,10 +707,10 @@
   <sheetData>
     <row r="1" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -756,7 +756,7 @@
       <c r="Q4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="T4" s="5" t="s">
         <v>54</v>
       </c>
       <c r="U4" s="4" t="s">
@@ -770,10 +770,10 @@
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
     </row>
     <row r="6" spans="2:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
@@ -782,13 +782,13 @@
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="4" t="s">
         <v>13</v>
@@ -799,7 +799,7 @@
       <c r="J6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="10" t="s">
         <v>45</v>
       </c>
       <c r="L6" s="4"/>
@@ -813,7 +813,7 @@
       <c r="P6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q6" s="13" t="s">
+      <c r="Q6" s="11" t="s">
         <v>22</v>
       </c>
       <c r="T6" s="4" t="s">
@@ -825,7 +825,7 @@
       <c r="V6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="W6" s="12" t="s">
+      <c r="W6" s="10" t="s">
         <v>60</v>
       </c>
     </row>
@@ -839,7 +839,7 @@
       <c r="D7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="1"/>
@@ -853,7 +853,7 @@
       <c r="J7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="10" t="s">
         <v>46</v>
       </c>
       <c r="L7" s="4"/>
@@ -867,7 +867,7 @@
       <c r="P7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q7" s="13" t="s">
+      <c r="Q7" s="11" t="s">
         <v>22</v>
       </c>
       <c r="T7" s="4" t="s">
@@ -879,7 +879,7 @@
       <c r="V7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="W7" s="12" t="s">
+      <c r="W7" s="10" t="s">
         <v>61</v>
       </c>
     </row>
@@ -893,7 +893,7 @@
       <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="10" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="1"/>
@@ -907,7 +907,7 @@
       <c r="J8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="10" t="s">
         <v>47</v>
       </c>
       <c r="L8" s="4"/>
@@ -921,7 +921,7 @@
       <c r="P8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="13" t="s">
+      <c r="Q8" s="11" t="s">
         <v>22</v>
       </c>
       <c r="T8" s="4" t="s">
@@ -933,7 +933,7 @@
       <c r="V8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="W8" s="12" t="s">
+      <c r="W8" s="10" t="s">
         <v>62</v>
       </c>
     </row>
@@ -947,12 +947,12 @@
       <c r="D9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="8" t="s">
         <v>14</v>
       </c>
       <c r="I9" s="4" t="s">
@@ -961,7 +961,7 @@
       <c r="J9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="10" t="s">
         <v>48</v>
       </c>
       <c r="L9" s="4"/>
@@ -975,7 +975,7 @@
       <c r="P9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q9" s="13" t="s">
+      <c r="Q9" s="11" t="s">
         <v>22</v>
       </c>
       <c r="T9" s="4" t="s">
@@ -987,7 +987,7 @@
       <c r="V9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="W9" s="12" t="s">
+      <c r="W9" s="10" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1001,12 +1001,12 @@
       <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="10" t="s">
         <v>29</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I10" s="4" t="s">
@@ -1015,7 +1015,7 @@
       <c r="J10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="10" t="s">
         <v>49</v>
       </c>
       <c r="L10" s="4"/>
@@ -1029,7 +1029,7 @@
       <c r="P10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q10" s="13" t="s">
+      <c r="Q10" s="11" t="s">
         <v>22</v>
       </c>
       <c r="T10" s="4" t="s">
@@ -1041,7 +1041,7 @@
       <c r="V10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="W10" s="12" t="s">
+      <c r="W10" s="10" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1055,12 +1055,12 @@
       <c r="D11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="10" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="4" t="s">
@@ -1069,7 +1069,7 @@
       <c r="J11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="10" t="s">
         <v>50</v>
       </c>
       <c r="L11" s="4"/>
@@ -1083,13 +1083,21 @@
       <c r="P11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" s="13" t="s">
+      <c r="Q11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="13"/>
+      <c r="T11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W11" s="11" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="12" spans="2:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
@@ -1101,12 +1109,12 @@
       <c r="D12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="I12" s="4" t="s">
@@ -1115,7 +1123,7 @@
       <c r="J12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="10" t="s">
         <v>51</v>
       </c>
       <c r="L12" s="4"/>
@@ -1129,16 +1137,16 @@
       <c r="P12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q12" s="13" t="s">
+      <c r="Q12" s="11" t="s">
         <v>22</v>
       </c>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="4"/>
-      <c r="W12" s="13"/>
+      <c r="W12" s="11"/>
     </row>
     <row r="13" spans="2:23" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>53</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -1147,10 +1155,22 @@
       <c r="J13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="10" t="s">
         <v>52</v>
       </c>
       <c r="L13" s="3"/>
+      <c r="N13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q13" s="11" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1163,38 +1183,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{835DB90F-02B5-433E-BF37-83E02E0A67CF}">
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="18" t="s">
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="19"/>
-    </row>
-    <row r="5" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="11" t="s">
+      <c r="C3" s="16"/>
+    </row>
+    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>